<commit_message>
house keeping of expansion box files and model updates
</commit_message>
<xml_diff>
--- a/CaseStudies/SimulinkOpal/Canary_OpalReady/Canary_UDP_Mapping.xlsx
+++ b/CaseStudies/SimulinkOpal/Canary_OpalReady/Canary_UDP_Mapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t>N/A</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>F1 Motor Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">Fuel usage </t>
@@ -349,18 +346,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -400,36 +395,21 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -443,9 +423,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -752,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,788 +747,783 @@
     <col min="8" max="8" width="49.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41">
+      <c r="C1" s="34">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="23">
-        <v>1</v>
-      </c>
-      <c r="E4" s="23">
-        <v>1</v>
-      </c>
-      <c r="F4" s="23">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="21">
+        <v>1</v>
+      </c>
+      <c r="E4" s="21">
+        <v>1</v>
+      </c>
+      <c r="F4" s="21">
         <f t="shared" ref="F4:F30" si="0">RIGHT(C4,2)/8*D4*E4*$C$1</f>
         <v>10</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="4" t="s">
+      <c r="G4" s="21"/>
+      <c r="H4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="24">
-        <v>1</v>
-      </c>
-      <c r="E5" s="24">
+      <c r="C5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="22">
+        <v>1</v>
+      </c>
+      <c r="E5" s="22">
         <v>3</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="23">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="G5" s="24">
-        <v>1</v>
-      </c>
-      <c r="H5" s="12" t="s">
+      <c r="G5" s="22">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="26">
-        <v>1</v>
-      </c>
-      <c r="E6" s="26">
+      <c r="C6" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="24">
+        <v>1</v>
+      </c>
+      <c r="E6" s="24">
         <v>20</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="25">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="G6" s="26">
-        <v>10</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="24">
+        <v>10</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="26">
-        <v>1</v>
-      </c>
-      <c r="E7" s="26">
+      <c r="C7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="24">
+        <v>1</v>
+      </c>
+      <c r="E7" s="24">
         <v>20</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="25">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="G7" s="26">
-        <v>10</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="G7" s="24">
+        <v>10</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="26">
-        <v>1</v>
-      </c>
-      <c r="E8" s="26">
+      <c r="C8" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="24">
+        <v>1</v>
+      </c>
+      <c r="E8" s="24">
         <v>20</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="25">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="24">
         <v>100</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="26">
-        <v>1</v>
-      </c>
-      <c r="E9" s="26">
+      <c r="C9" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="24">
+        <v>1</v>
+      </c>
+      <c r="E9" s="24">
         <v>20</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="25">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="24">
         <v>100</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="26">
-        <v>1</v>
-      </c>
-      <c r="E10" s="26">
+      <c r="C10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="24">
+        <v>1</v>
+      </c>
+      <c r="E10" s="24">
         <v>20</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="25">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="G10" s="26">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6" t="s">
+      <c r="G10" s="24">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="24">
-        <v>1</v>
-      </c>
-      <c r="E11" s="24">
+      <c r="C11" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="22">
         <v>1</v>
       </c>
       <c r="F11" s="25">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G11" s="24">
-        <v>1</v>
-      </c>
-      <c r="H11" s="13" t="s">
+      <c r="G11" s="22">
+        <v>1</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="26">
+        <v>1</v>
+      </c>
+      <c r="E12" s="27">
+        <v>1</v>
+      </c>
+      <c r="F12" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G12" s="26">
+        <v>100</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="28">
-        <v>1</v>
-      </c>
-      <c r="E12" s="29">
-        <v>1</v>
-      </c>
-      <c r="F12" s="30">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G12" s="28">
+      <c r="C13" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="26">
+        <v>1</v>
+      </c>
+      <c r="E13" s="27">
+        <v>1</v>
+      </c>
+      <c r="F13" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G13" s="26">
         <v>100</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H13" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="28">
-        <v>1</v>
-      </c>
-      <c r="E13" s="29">
-        <v>1</v>
-      </c>
-      <c r="F13" s="30">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G13" s="28">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="28">
+        <v>1</v>
+      </c>
+      <c r="E14" s="29">
+        <v>1</v>
+      </c>
+      <c r="F14" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G14" s="28">
         <v>100</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H14" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="31">
-        <v>1</v>
-      </c>
-      <c r="E14" s="32">
-        <v>1</v>
-      </c>
-      <c r="F14" s="33">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G14" s="31">
+      <c r="B15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="28">
+        <v>1</v>
+      </c>
+      <c r="E15" s="29">
+        <v>1</v>
+      </c>
+      <c r="F15" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G15" s="28">
         <v>100</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="H15" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="31">
-        <v>1</v>
-      </c>
-      <c r="E15" s="32">
-        <v>1</v>
-      </c>
-      <c r="F15" s="33">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G15" s="31">
+      <c r="B16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="28">
+        <v>1</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G16" s="28">
         <v>100</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="H16" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="31">
-        <v>1</v>
-      </c>
-      <c r="E16" s="32">
-        <v>1</v>
-      </c>
-      <c r="F16" s="33">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G16" s="31">
+      <c r="B17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="28">
+        <v>1</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G17" s="28">
         <v>100</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H17" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="28">
+        <v>1</v>
+      </c>
+      <c r="E18" s="29">
+        <v>1</v>
+      </c>
+      <c r="F18" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G18" s="28">
+        <v>100</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="28">
+        <v>1</v>
+      </c>
+      <c r="E19" s="29">
+        <v>1</v>
+      </c>
+      <c r="F19" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G19" s="28">
+        <v>100</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="28">
+        <v>1</v>
+      </c>
+      <c r="E20" s="29">
+        <v>1</v>
+      </c>
+      <c r="F20" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G20" s="28">
+        <v>100</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="31">
-        <v>1</v>
-      </c>
-      <c r="E17" s="32">
-        <v>1</v>
-      </c>
-      <c r="F17" s="33">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G17" s="31">
+      <c r="C21" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="28">
+        <v>1</v>
+      </c>
+      <c r="E21" s="29">
+        <v>1</v>
+      </c>
+      <c r="F21" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G21" s="28">
         <v>100</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H21" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="31">
-        <v>1</v>
-      </c>
-      <c r="E18" s="32">
-        <v>1</v>
-      </c>
-      <c r="F18" s="33">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G18" s="31">
+      <c r="B22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="28">
+        <v>1</v>
+      </c>
+      <c r="E22" s="29">
+        <v>1</v>
+      </c>
+      <c r="F22" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G22" s="28">
         <v>100</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H22" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="31">
-        <v>1</v>
-      </c>
-      <c r="E19" s="32">
-        <v>1</v>
-      </c>
-      <c r="F19" s="33">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G19" s="31">
-        <v>100</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="31">
-        <v>1</v>
-      </c>
-      <c r="E20" s="32">
-        <v>1</v>
-      </c>
-      <c r="F20" s="33">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G20" s="31">
-        <v>100</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="31">
-        <v>1</v>
-      </c>
-      <c r="E21" s="32">
-        <v>1</v>
-      </c>
-      <c r="F21" s="33">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G21" s="31">
-        <v>100</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="31">
-        <v>1</v>
-      </c>
-      <c r="E22" s="32">
-        <v>1</v>
-      </c>
-      <c r="F22" s="33">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G22" s="31">
-        <v>100</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="34">
-        <v>1</v>
-      </c>
-      <c r="E23" s="34">
-        <v>1</v>
-      </c>
-      <c r="F23" s="35">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G23" s="34">
-        <v>1</v>
-      </c>
-      <c r="H23" s="17" t="s">
+      <c r="C23" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="30">
+        <v>1</v>
+      </c>
+      <c r="E23" s="30">
+        <v>1</v>
+      </c>
+      <c r="F23" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G23" s="30">
+        <v>1</v>
+      </c>
+      <c r="H23" s="15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="24">
+      <c r="C24" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="22">
+        <v>1</v>
+      </c>
+      <c r="E24" s="22">
         <v>1</v>
       </c>
       <c r="F24" s="25">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G24" s="24">
-        <v>1</v>
-      </c>
-      <c r="H24" s="13" t="s">
+      <c r="G24" s="22">
+        <v>1</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="36">
-        <v>1</v>
-      </c>
-      <c r="E25" s="36">
-        <v>1</v>
-      </c>
-      <c r="F25" s="37">
-        <f>RIGHT(C25,2)/8*D25*E25*$C$1</f>
-        <v>10</v>
-      </c>
-      <c r="G25" s="36">
+      <c r="C25" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="31">
+        <v>1</v>
+      </c>
+      <c r="E25" s="31">
+        <v>1</v>
+      </c>
+      <c r="F25" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G25" s="31">
         <v>1000</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="36">
-        <v>1</v>
-      </c>
-      <c r="E26" s="36">
-        <v>1</v>
-      </c>
-      <c r="F26" s="37">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G26" s="36">
-        <v>1</v>
-      </c>
-      <c r="H26" s="14" t="s">
+      <c r="C26" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="31">
+        <v>1</v>
+      </c>
+      <c r="E26" s="31">
+        <v>1</v>
+      </c>
+      <c r="F26" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G26" s="31">
+        <v>1</v>
+      </c>
+      <c r="H26" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="36">
-        <v>1</v>
-      </c>
-      <c r="E27" s="36">
-        <v>1</v>
-      </c>
-      <c r="F27" s="37">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G27" s="36">
-        <v>1</v>
-      </c>
-      <c r="H27" s="14" t="s">
+      <c r="C27" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="31">
+        <v>1</v>
+      </c>
+      <c r="E27" s="31">
+        <v>1</v>
+      </c>
+      <c r="F27" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G27" s="31">
+        <v>1</v>
+      </c>
+      <c r="H27" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="J27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="38">
-        <v>1</v>
-      </c>
-      <c r="E28" s="38">
+      <c r="C28" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="32">
+        <v>1</v>
+      </c>
+      <c r="E28" s="32">
         <v>3</v>
       </c>
-      <c r="F28" s="39">
+      <c r="F28" s="25">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="G28" s="38">
-        <v>1</v>
-      </c>
-      <c r="H28" s="20" t="s">
+      <c r="G28" s="32">
+        <v>1</v>
+      </c>
+      <c r="H28" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="40">
-        <v>1</v>
-      </c>
-      <c r="E29" s="40">
-        <v>1</v>
-      </c>
-      <c r="F29" s="23">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G29" s="40"/>
-      <c r="H29" s="5" t="s">
+      <c r="C29" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="33">
+        <v>1</v>
+      </c>
+      <c r="E29" s="33">
+        <v>1</v>
+      </c>
+      <c r="F29" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="33"/>
+      <c r="H29" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
+    <row r="30" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="44">
-        <v>1</v>
-      </c>
-      <c r="E30" s="44">
-        <v>1</v>
-      </c>
-      <c r="F30" s="45">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G30" s="44"/>
-      <c r="H30" s="46" t="s">
+      <c r="C30" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="37">
+        <v>1</v>
+      </c>
+      <c r="E30" s="37">
+        <v>1</v>
+      </c>
+      <c r="F30" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G30" s="37"/>
+      <c r="H30" s="38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E31" s="42">
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E31" s="35">
         <f>SUM(E6:E30)+E4+D5*E5</f>
         <v>126</v>
       </c>
-      <c r="F31" s="43"/>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
+      <c r="F31" s="36"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
     </row>
     <row r="33" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="42">
+      <c r="F33" s="35">
         <f>SUM(F4:F32)</f>
         <v>1260</v>
       </c>

</xml_diff>